<commit_message>
add the new version of the BDRK=BDRK+BLUR+DEAC
</commit_message>
<xml_diff>
--- a/try3/sppFilter/assSpp.xlsx
+++ b/try3/sppFilter/assSpp.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickg/Documents/jobs/nmfs/sppComp/try3/sppFilter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A173619A-F6DE-D044-AE03-F8AA4AB1D5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D5ED4F-143C-5142-AC09-AA6F16902D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="500" windowWidth="21000" windowHeight="33100" activeTab="1"/>
+    <workbookView xWindow="3280" yWindow="-17500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fmpSpp" sheetId="1" r:id="rId1"/>
@@ -1982,7 +1982,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2816,7 +2816,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F230"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
@@ -6616,11 +6616,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="A7" sqref="A7:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6715,10 +6715,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="C7" t="s">
         <v>516</v>
@@ -6727,7 +6727,7 @@
         <v>47</v>
       </c>
       <c r="F7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G7" t="s">
         <v>109</v>

</xml_diff>